<commit_message>
use star character to represent dongling
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t xml:space="preserve">序号</t>
   </si>
@@ -43,9 +43,6 @@
     <t xml:space="preserve">坝上风云</t>
   </si>
   <si>
-    <t xml:space="preserve">合计</t>
-  </si>
-  <si>
     <t xml:space="preserve">东灵完成</t>
   </si>
   <si>
@@ -55,22 +52,22 @@
     <t xml:space="preserve">甲</t>
   </si>
   <si>
+    <t xml:space="preserve">是</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">乙</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">丙</t>
+  </si>
+  <si>
     <t xml:space="preserve">否</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">乙</t>
-  </si>
-  <si>
-    <t xml:space="preserve">是</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">丙</t>
   </si>
   <si>
     <t xml:space="preserve">4</t>
@@ -387,13 +384,13 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="8.03"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="8" style="2" width="8.03"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -418,48 +415,44 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>4</v>
@@ -468,7 +461,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F3" s="5" t="n">
         <v>2</v>
@@ -476,49 +469,45 @@
       <c r="G3" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H3" s="5" t="n">
-        <v>11</v>
-      </c>
+      <c r="H3" s="5"/>
       <c r="I3" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" s="5" t="n">
         <v>2</v>
       </c>
@@ -532,27 +521,25 @@
         <v>1</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>3</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="H5" s="5"/>
       <c r="I5" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="C6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6" s="5" t="n">
         <v>2</v>
@@ -563,22 +550,20 @@
       <c r="G6" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H6" s="5" t="n">
-        <v>2</v>
-      </c>
+      <c r="H6" s="5"/>
       <c r="I6" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="C7" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>0</v>
@@ -592,19 +577,17 @@
       <c r="G7" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="5" t="n">
-        <v>7</v>
-      </c>
+      <c r="H7" s="5"/>
       <c r="I7" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>4</v>
@@ -621,25 +604,23 @@
       <c r="G8" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="5" t="n">
-        <v>8</v>
-      </c>
+      <c r="H8" s="5"/>
       <c r="I8" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="C9" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>0</v>
@@ -648,22 +629,20 @@
         <v>1</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5" t="n">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H9" s="5"/>
       <c r="I9" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="C10" s="5" t="n">
         <v>0</v>
       </c>
@@ -674,24 +653,22 @@
         <v>2</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H10" s="5" t="n">
-        <v>2</v>
-      </c>
+      <c r="H10" s="5"/>
       <c r="I10" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="C11" s="5" t="n">
         <v>2</v>
@@ -708,20 +685,18 @@
       <c r="G11" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H11" s="5" t="n">
-        <v>7</v>
-      </c>
+      <c r="H11" s="5"/>
       <c r="I11" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C12" s="5" t="n">
         <v>2</v>
       </c>
@@ -737,20 +712,18 @@
       <c r="G12" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H12" s="5" t="n">
-        <v>7</v>
-      </c>
+      <c r="H12" s="5"/>
       <c r="I12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C13" s="5" t="n">
         <v>0</v>
       </c>
@@ -766,25 +739,23 @@
       <c r="G13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H13" s="5" t="n">
-        <v>2</v>
-      </c>
+      <c r="H13" s="5"/>
       <c r="I13" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C14" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>0</v>
@@ -793,27 +764,25 @@
         <v>0</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="5" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H14" s="5"/>
       <c r="I14" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C15" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>0</v>
@@ -822,13 +791,11 @@
         <v>0</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5" t="n">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H15" s="5"/>
       <c r="I15" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>